<commit_message>
Documentation and testing before release
</commit_message>
<xml_diff>
--- a/examples/process_123.xlsx
+++ b/examples/process_123.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F027649-B096-4745-B085-F941ACED837F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235E01DB-F3AC-4C25-842D-4527DC357367}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="steps" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>step_id</t>
   </si>
@@ -514,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -599,9 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>